<commit_message>
New File PP Regression5
</commit_message>
<xml_diff>
--- a/Test_Planner/SAP_Test_Planner_Healthcheck.xlsx
+++ b/Test_Planner/SAP_Test_Planner_Healthcheck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\Test_Planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3665C963-739E-49AE-ABF8-121709C34B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F79E71-3038-4A91-9637-2255C6A088E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3F52AFC6-D99D-4450-AD0F-1227D9226E9B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="55">
   <si>
     <t>SuteName</t>
   </si>
@@ -167,6 +167,42 @@
   </si>
   <si>
     <t>Cancelling Order via JSON File and Fetch the Status</t>
+  </si>
+  <si>
+    <t>Create PP with Invalid Society</t>
+  </si>
+  <si>
+    <t>Create PP with Invalid Article Type</t>
+  </si>
+  <si>
+    <t>Create PP with Invalid Editorial</t>
+  </si>
+  <si>
+    <t>Create PP with Invalid Referal</t>
+  </si>
+  <si>
+    <t>Create PP with Invalid CountryCode</t>
+  </si>
+  <si>
+    <t>Create PP with Invalid MailId</t>
+  </si>
+  <si>
+    <t>NC_OP_16</t>
+  </si>
+  <si>
+    <t>NC_OP_17</t>
+  </si>
+  <si>
+    <t>NC_OP_18</t>
+  </si>
+  <si>
+    <t>NC_OP_19</t>
+  </si>
+  <si>
+    <t>NC_OP_20</t>
+  </si>
+  <si>
+    <t>NC_OP_21</t>
   </si>
 </sst>
 </file>
@@ -272,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -285,6 +321,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -655,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34CF3798-65B8-4491-99A4-6813C24FCF65}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -990,6 +1027,108 @@
       </c>
       <c r="E19" s="6" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="8">
+        <v>5393960</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="8">
+        <v>5393961</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="8">
+        <v>5393962</v>
+      </c>
+      <c r="E22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="8">
+        <v>5393963</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="8">
+        <v>5393964</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="8">
+        <v>5393965</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1012,7 +1151,7 @@
       <formula>COUNTIF(G$95:G$140,#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E16 C20:E1048576 D17:E19">
+  <conditionalFormatting sqref="E3:E16 D17:E19 C20:E1048576">
     <cfRule type="expression" dxfId="0" priority="3573">
       <formula>COUNTIF(#REF!,#REF!)</formula>
     </cfRule>
@@ -1023,7 +1162,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B19" xr:uid="{DE21EE38-54D7-44B6-A9E8-B480FE2F7BC6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B25" xr:uid="{DE21EE38-54D7-44B6-A9E8-B480FE2F7BC6}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1033,18 +1172,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1251,14 +1390,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9A5492E-A32A-41EE-AAEE-6E8BE77D7028}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34FB7BFF-CBF3-491F-A454-15CC4708CCB1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -1271,6 +1402,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="a577898b-6855-4c00-94c2-65f3a1a2604e"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9A5492E-A32A-41EE-AAEE-6E8BE77D7028}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
New File PP Regression6
</commit_message>
<xml_diff>
--- a/Test_Planner/SAP_Test_Planner_Healthcheck.xlsx
+++ b/Test_Planner/SAP_Test_Planner_Healthcheck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\Test_Planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F79E71-3038-4A91-9637-2255C6A088E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FCF1A2-E5E5-412C-9022-84A4562F299F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3F52AFC6-D99D-4450-AD0F-1227D9226E9B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="56">
   <si>
     <t>SuteName</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>NC_OP_21</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -308,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -322,7 +325,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -983,7 +985,7 @@
         <v>6</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>38</v>
@@ -1000,7 +1002,7 @@
         <v>6</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>39</v>
@@ -1017,7 +1019,7 @@
         <v>6</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>37</v>
@@ -1036,7 +1038,7 @@
       <c r="B20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>49</v>
       </c>
       <c r="D20" s="8">
@@ -1053,7 +1055,7 @@
       <c r="B21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="8" t="s">
         <v>50</v>
       </c>
       <c r="D21" s="8">
@@ -1070,7 +1072,7 @@
       <c r="B22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="8" t="s">
         <v>51</v>
       </c>
       <c r="D22" s="8">
@@ -1087,7 +1089,7 @@
       <c r="B23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="8" t="s">
         <v>52</v>
       </c>
       <c r="D23" s="8">
@@ -1104,7 +1106,7 @@
       <c r="B24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="8" t="s">
         <v>53</v>
       </c>
       <c r="D24" s="8">
@@ -1121,7 +1123,7 @@
       <c r="B25" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="8" t="s">
         <v>54</v>
       </c>
       <c r="D25" s="8">
@@ -1152,12 +1154,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E16 D17:E19 C20:E1048576">
-    <cfRule type="expression" dxfId="0" priority="3573">
+    <cfRule type="expression" dxfId="1" priority="3573">
       <formula>COUNTIF(#REF!,#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="expression" dxfId="1" priority="3642">
+    <cfRule type="expression" dxfId="0" priority="3642">
       <formula>COUNTIF(#REF!,#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1172,18 +1174,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1390,6 +1392,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9A5492E-A32A-41EE-AAEE-6E8BE77D7028}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34FB7BFF-CBF3-491F-A454-15CC4708CCB1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -1402,14 +1412,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="a577898b-6855-4c00-94c2-65f3a1a2604e"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9A5492E-A32A-41EE-AAEE-6E8BE77D7028}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
UI Validations added V.12
</commit_message>
<xml_diff>
--- a/Test_Planner/SAP_Test_Planner_Healthcheck.xlsx
+++ b/Test_Planner/SAP_Test_Planner_Healthcheck.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\Test_Planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D5F6D9-507D-4FB3-ACD5-FAA549B534EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61892E80-EFF1-4406-AF05-B50A5F402089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="380" windowWidth="19200" windowHeight="10200" xr2:uid="{3F52AFC6-D99D-4450-AD0F-1227D9226E9B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3F52AFC6-D99D-4450-AD0F-1227D9226E9B}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="60">
   <si>
     <t>SuteName</t>
   </si>
@@ -206,6 +206,18 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>NC_OP_22</t>
+  </si>
+  <si>
+    <t>NC_OP_23</t>
+  </si>
+  <si>
+    <t>Create PP Society discount with Rejected</t>
+  </si>
+  <si>
+    <t>Create PP Society discount with Withdrawn</t>
   </si>
 </sst>
 </file>
@@ -311,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -325,6 +337,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -694,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34CF3798-65B8-4491-99A4-6813C24FCF65}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1131,6 +1147,40 @@
       </c>
       <c r="E25" s="6" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="10">
+        <v>5397361</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="10">
+        <v>5397362</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1164,7 +1214,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B25" xr:uid="{DE21EE38-54D7-44B6-A9E8-B480FE2F7BC6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B27" xr:uid="{DE21EE38-54D7-44B6-A9E8-B480FE2F7BC6}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1180,6 +1230,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009EB318C388A6B04FB5EA4B6A454DD04D" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="529c52af2e5f736fd7766b468ba66b9f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a577898b-6855-4c00-94c2-65f3a1a2604e" xmlns:ns4="f8d9bec8-ea51-4f0f-8110-f49fc874611e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bb04426f2fa1e3093e624188e4495695" ns3:_="" ns4:_="">
     <xsd:import namespace="a577898b-6855-4c00-94c2-65f3a1a2604e"/>
@@ -1382,15 +1441,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34FB7BFF-CBF3-491F-A454-15CC4708CCB1}">
   <ds:schemaRefs>
@@ -1409,6 +1459,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9A5492E-A32A-41EE-AAEE-6E8BE77D7028}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4CBA780-8BAE-47D7-A333-9374A3A80872}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1425,12 +1483,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9A5492E-A32A-41EE-AAEE-6E8BE77D7028}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
UI Validations added V.46
</commit_message>
<xml_diff>
--- a/Test_Planner/SAP_Test_Planner_Healthcheck.xlsx
+++ b/Test_Planner/SAP_Test_Planner_Healthcheck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchinnasam\OneDrive\Documents\SAP Test Automation\SAP-Test-Automation\Test_Planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D2DF3B-8C00-407C-92AD-A5067268C9C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5446D269-90CE-437F-9404-40E4CF3F6C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3F52AFC6-D99D-4450-AD0F-1227D9226E9B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="55">
   <si>
     <t>SuteName</t>
   </si>
@@ -151,24 +151,6 @@
     <t>Create PP with Manual override required value as Yes</t>
   </si>
   <si>
-    <t>VA_CO_03</t>
-  </si>
-  <si>
-    <t>VA_CO_01</t>
-  </si>
-  <si>
-    <t>VA_CO_02</t>
-  </si>
-  <si>
-    <t>Create Order via JSON File and Fetch the Status</t>
-  </si>
-  <si>
-    <t>Validate the Values in DBS and download the PDF</t>
-  </si>
-  <si>
-    <t>Cancelling Order via JSON File and Fetch the Status</t>
-  </si>
-  <si>
     <t>Create PP with Invalid Society</t>
   </si>
   <si>
@@ -203,9 +185,6 @@
   </si>
   <si>
     <t>NC_OP_21</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>NC_OP_22</t>
@@ -329,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -343,7 +322,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -713,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34CF3798-65B8-4491-99A4-6813C24FCF65}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1004,16 +982,16 @@
         <v>6</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>38</v>
+        <v>4</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="D17" s="8">
-        <v>5392267</v>
+        <v>5393960</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -1021,16 +999,16 @@
         <v>6</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>39</v>
+        <v>4</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="D18" s="8">
-        <v>5392268</v>
+        <v>5393961</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -1038,16 +1016,16 @@
         <v>6</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>37</v>
+        <v>4</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="D19" s="8">
-        <v>5392269</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>42</v>
+        <v>5393962</v>
+      </c>
+      <c r="E19" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -1058,13 +1036,13 @@
         <v>4</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D20" s="8">
-        <v>5393960</v>
+        <v>5393963</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1075,13 +1053,13 @@
         <v>4</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D21" s="8">
-        <v>5393961</v>
+        <v>5393964</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -1092,13 +1070,13 @@
         <v>4</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D22" s="8">
-        <v>5393962</v>
-      </c>
-      <c r="E22" t="s">
-        <v>45</v>
+        <v>5393965</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1109,13 +1087,13 @@
         <v>4</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D23" s="8">
-        <v>5393963</v>
+        <v>5397361</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -1126,13 +1104,13 @@
         <v>4</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D24" s="8">
-        <v>5393964</v>
+        <v>5397362</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1146,61 +1124,10 @@
         <v>54</v>
       </c>
       <c r="D25" s="8">
-        <v>5393965</v>
+        <v>5400136</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="8">
-        <v>5397361</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="8">
-        <v>5397362</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D28" s="9">
-        <v>5400136</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1220,10 +1147,10 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
     <cfRule type="expression" dxfId="2" priority="3641">
-      <formula>COUNTIF(G$92:G$137,#REF!)</formula>
+      <formula>COUNTIF(G$89:G$134,#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E16 D17:E19 C20:E1048576">
+  <conditionalFormatting sqref="E3:E16 C17:E1048576">
     <cfRule type="expression" dxfId="1" priority="3573">
       <formula>COUNTIF(#REF!,#REF!)</formula>
     </cfRule>
@@ -1234,7 +1161,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B28" xr:uid="{DE21EE38-54D7-44B6-A9E8-B480FE2F7BC6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B25" xr:uid="{DE21EE38-54D7-44B6-A9E8-B480FE2F7BC6}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1250,6 +1177,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009EB318C388A6B04FB5EA4B6A454DD04D" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="529c52af2e5f736fd7766b468ba66b9f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a577898b-6855-4c00-94c2-65f3a1a2604e" xmlns:ns4="f8d9bec8-ea51-4f0f-8110-f49fc874611e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bb04426f2fa1e3093e624188e4495695" ns3:_="" ns4:_="">
     <xsd:import namespace="a577898b-6855-4c00-94c2-65f3a1a2604e"/>
@@ -1452,15 +1388,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34FB7BFF-CBF3-491F-A454-15CC4708CCB1}">
   <ds:schemaRefs>
@@ -1479,6 +1406,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9A5492E-A32A-41EE-AAEE-6E8BE77D7028}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4CBA780-8BAE-47D7-A333-9374A3A80872}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1495,12 +1430,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9A5492E-A32A-41EE-AAEE-6E8BE77D7028}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>